<commit_message>
Created a copy of the RSE settings file (i.e. ORIGINAL).
</commit_message>
<xml_diff>
--- a/Settings/datafeeds_settings/df_RSE_settings.xlsx
+++ b/Settings/datafeeds_settings/df_RSE_settings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,16 +474,16 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -500,7 +500,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -514,12 +514,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -530,7 +530,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -555,7 +555,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -563,7 +563,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -577,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -585,7 +585,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -593,15 +593,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -610,15 +610,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -628,15 +628,15 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -646,15 +646,15 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -664,15 +664,15 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -682,15 +682,15 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -700,15 +700,15 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -718,15 +718,15 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -736,15 +736,15 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -754,15 +754,15 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -771,15 +771,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -788,15 +788,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -805,15 +805,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -822,15 +822,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -839,15 +839,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -856,15 +856,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -873,15 +873,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -890,15 +890,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -907,15 +907,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -924,15 +924,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -941,15 +941,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -958,15 +958,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -975,15 +975,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -992,15 +992,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B34">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1009,15 +1009,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B35">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1026,15 +1026,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1043,15 +1043,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D37">
         <v>1</v>

</xml_diff>